<commit_message>
Adição e formatação de currículos e correção do Cronograma
</commit_message>
<xml_diff>
--- a/docs/Project Docs/STE_CP_CronogramaDoProjeto.xlsx
+++ b/docs/Project Docs/STE_CP_CronogramaDoProjeto.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" codeName="EstaPasta_de_trabalho" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma + Diagrama de Gantt" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="119">
   <si>
     <t>Real</t>
   </si>
@@ -353,9 +353,6 @@
     <t>TASK-07</t>
   </si>
   <si>
-    <t>Iniciada</t>
-  </si>
-  <si>
     <t>Preparar base de dados para persistência de usuários. Ao final dessa tarefa desse ser possível acessar um banco de dados (remoto) e buscar dados de usuários com base no email (login). Os cripts usados para criar o banco devem ser inseridos por meio de documento no diretório de documentos do código. As senhas de acesso ao servidor mysql devem estar documentadas no documento de senhas. Dica: usar conta gratuita da amazon para criar instância grátis, instalar mysql, e criar banco. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
   </si>
   <si>
@@ -422,9 +419,6 @@
       </rPr>
       <t>Sprint 2</t>
     </r>
-  </si>
-  <si>
-    <t>Em espera</t>
   </si>
   <si>
     <t>Criar endpoints/views na aplicação para um usuário recuperar a senha, um e-mail deve ser enviado para o usuário que terá que redefinir sua senha. Endpoints devem ser documentados no documento de endpoints. Decisões relativas a aspectos internos dessa tarefa podem ser decididos pelo implementador.</t>
@@ -665,7 +659,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -740,6 +734,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -874,7 +880,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1103,6 +1109,9 @@
     <xf numFmtId="14" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1121,8 +1130,11 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -1136,7 +1148,217 @@
     <cellStyle name="Project Headers" xfId="4"/>
     <cellStyle name="Título 1" xfId="1" builtinId="16" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="48">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF004080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF004080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF004080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF004080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF004080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF004080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF004080"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -1451,6 +1673,7 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFF3300"/>
       <color rgb="FFFFFFFF"/>
       <color rgb="FF004080"/>
       <color rgb="FF00407E"/>
@@ -2047,8 +2270,8 @@
   </sheetPr>
   <dimension ref="B1:HE701"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
@@ -2115,14 +2338,14 @@
       <c r="AG1" s="13"/>
     </row>
     <row r="2" spans="2:213" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="71" t="s">
+      <c r="B2" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
       <c r="H2" s="50" t="s">
         <v>3</v>
       </c>
@@ -2152,12 +2375,12 @@
       <c r="AG2" s="6"/>
     </row>
     <row r="3" spans="2:213" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -2177,12 +2400,12 @@
       <c r="AG3" s="6"/>
     </row>
     <row r="4" spans="2:213" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
+      <c r="B4" s="72"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
       <c r="H4" s="50" t="s">
         <v>7</v>
       </c>
@@ -2220,12 +2443,12 @@
       <c r="AT4" s="5"/>
     </row>
     <row r="5" spans="2:213" ht="17.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B5" s="71"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -3094,7 +3317,7 @@
       </c>
       <c r="E7" s="43">
         <f>(J7-H7)+1</f>
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="F7" s="36">
         <f>AVERAGE($F$9:$F$48)</f>
@@ -3114,7 +3337,7 @@
       </c>
       <c r="J7" s="37">
         <f>LARGE($J$8:$J$47,1)</f>
-        <v>42510</v>
+        <v>42554</v>
       </c>
       <c r="K7" s="37"/>
       <c r="L7" s="38"/>
@@ -3885,7 +4108,7 @@
         <v>42510</v>
       </c>
       <c r="K11" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L11" s="41" t="s">
         <v>34</v>
@@ -4122,7 +4345,7 @@
         <v>42510</v>
       </c>
       <c r="K12" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L12" s="41" t="s">
         <v>34</v>
@@ -4359,7 +4582,7 @@
         <v>42510</v>
       </c>
       <c r="K13" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L13" s="41" t="s">
         <v>34</v>
@@ -4596,7 +4819,7 @@
         <v>42510</v>
       </c>
       <c r="K14" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L14" s="41" t="s">
         <v>34</v>
@@ -4804,32 +5027,37 @@
       <c r="HE14" s="17"/>
     </row>
     <row r="15" spans="2:213" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
+      <c r="B15" s="34">
+        <v>2</v>
+      </c>
       <c r="C15" s="39" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="34">
         <v>2</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="E15" s="34">
+        <v>2</v>
+      </c>
       <c r="F15" s="40">
         <v>0</v>
       </c>
       <c r="G15" s="10">
-        <v>42503</v>
-      </c>
-      <c r="H15" s="10"/>
+        <v>42550</v>
+      </c>
+      <c r="H15" s="10">
+        <v>42550</v>
+      </c>
       <c r="I15" s="27">
         <f t="shared" ref="I15:I46" si="144">(G15+D15)-1</f>
-        <v>42504</v>
+        <v>42551</v>
       </c>
       <c r="J15" s="27">
         <f t="shared" si="143"/>
-        <v>-1</v>
-      </c>
-      <c r="K15" s="27" t="str">
-        <f t="shared" ca="1" si="141"/>
-        <v>Em atraso</v>
+        <v>42551</v>
+      </c>
+      <c r="K15" s="27" t="s">
+        <v>97</v>
       </c>
       <c r="L15" s="41" t="s">
         <v>34</v>
@@ -5037,32 +5265,37 @@
       <c r="HE15" s="17"/>
     </row>
     <row r="16" spans="2:213" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
+      <c r="B16" s="34">
+        <v>2</v>
+      </c>
       <c r="C16" s="39" t="s">
         <v>36</v>
       </c>
       <c r="D16" s="34">
         <v>2</v>
       </c>
-      <c r="E16" s="34"/>
+      <c r="E16" s="34">
+        <v>2</v>
+      </c>
       <c r="F16" s="40">
         <v>0</v>
       </c>
       <c r="G16" s="10">
-        <v>42503</v>
-      </c>
-      <c r="H16" s="10"/>
+        <v>42551</v>
+      </c>
+      <c r="H16" s="10">
+        <v>42551</v>
+      </c>
       <c r="I16" s="27">
         <f t="shared" si="144"/>
-        <v>42504</v>
+        <v>42552</v>
       </c>
       <c r="J16" s="27">
         <f t="shared" si="143"/>
-        <v>-1</v>
-      </c>
-      <c r="K16" s="27" t="str">
-        <f t="shared" ca="1" si="141"/>
-        <v>Em atraso</v>
+        <v>42552</v>
+      </c>
+      <c r="K16" s="27" t="s">
+        <v>97</v>
       </c>
       <c r="L16" s="41" t="s">
         <v>34</v>
@@ -5270,32 +5503,37 @@
       <c r="HE16" s="17"/>
     </row>
     <row r="17" spans="2:213" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="34"/>
+      <c r="B17" s="34">
+        <v>2</v>
+      </c>
       <c r="C17" s="39" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="34">
         <v>2</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="34">
+        <v>2</v>
+      </c>
       <c r="F17" s="40">
         <v>0</v>
       </c>
       <c r="G17" s="10">
-        <v>42503</v>
-      </c>
-      <c r="H17" s="10"/>
+        <v>42551</v>
+      </c>
+      <c r="H17" s="10">
+        <v>42551</v>
+      </c>
       <c r="I17" s="27">
         <f t="shared" si="144"/>
-        <v>42504</v>
+        <v>42552</v>
       </c>
       <c r="J17" s="27">
         <f t="shared" si="143"/>
-        <v>-1</v>
-      </c>
-      <c r="K17" s="27" t="str">
-        <f t="shared" ca="1" si="141"/>
-        <v>Em atraso</v>
+        <v>42552</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>97</v>
       </c>
       <c r="L17" s="41" t="s">
         <v>34</v>
@@ -5503,32 +5741,37 @@
       <c r="HE17" s="17"/>
     </row>
     <row r="18" spans="2:213" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="34"/>
+      <c r="B18" s="34">
+        <v>2</v>
+      </c>
       <c r="C18" s="39" t="s">
         <v>38</v>
       </c>
       <c r="D18" s="34">
-        <v>2</v>
-      </c>
-      <c r="E18" s="34"/>
+        <v>4</v>
+      </c>
+      <c r="E18" s="34">
+        <v>4</v>
+      </c>
       <c r="F18" s="40">
         <v>0</v>
       </c>
       <c r="G18" s="10">
-        <v>42503</v>
-      </c>
-      <c r="H18" s="10"/>
+        <v>42551</v>
+      </c>
+      <c r="H18" s="10">
+        <v>42551</v>
+      </c>
       <c r="I18" s="27">
         <f t="shared" si="144"/>
-        <v>42504</v>
+        <v>42554</v>
       </c>
       <c r="J18" s="27">
         <f t="shared" ref="J18:J46" si="145">(H18+E18)-1</f>
-        <v>-1</v>
-      </c>
-      <c r="K18" s="27" t="str">
-        <f t="shared" ref="K18:K46" ca="1" si="146">IF(F18=1,"Concluído",IF(AND(J18&lt;TODAY(),F18&lt;1),"Em atraso","Em andamento"))</f>
-        <v>Em atraso</v>
+        <v>42554</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>97</v>
       </c>
       <c r="L18" s="41" t="s">
         <v>34</v>
@@ -5736,32 +5979,37 @@
       <c r="HE18" s="17"/>
     </row>
     <row r="19" spans="2:213" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="34"/>
+      <c r="B19" s="34">
+        <v>2</v>
+      </c>
       <c r="C19" s="39" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="34">
         <v>2</v>
       </c>
-      <c r="E19" s="34"/>
+      <c r="E19" s="34">
+        <v>2</v>
+      </c>
       <c r="F19" s="40">
         <v>0</v>
       </c>
       <c r="G19" s="10">
-        <v>42503</v>
-      </c>
-      <c r="H19" s="10"/>
+        <v>42551</v>
+      </c>
+      <c r="H19" s="10">
+        <v>42551</v>
+      </c>
       <c r="I19" s="27">
         <f t="shared" si="144"/>
-        <v>42504</v>
+        <v>42552</v>
       </c>
       <c r="J19" s="27">
         <f t="shared" si="145"/>
-        <v>-1</v>
-      </c>
-      <c r="K19" s="27" t="str">
-        <f t="shared" ca="1" si="146"/>
-        <v>Em atraso</v>
+        <v>42552</v>
+      </c>
+      <c r="K19" s="27" t="s">
+        <v>97</v>
       </c>
       <c r="L19" s="41" t="s">
         <v>34</v>
@@ -5969,32 +6217,37 @@
       <c r="HE19" s="17"/>
     </row>
     <row r="20" spans="2:213" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="34"/>
+      <c r="B20" s="34">
+        <v>2</v>
+      </c>
       <c r="C20" s="39" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="34">
         <v>2</v>
       </c>
-      <c r="E20" s="34"/>
+      <c r="E20" s="34">
+        <v>2</v>
+      </c>
       <c r="F20" s="40">
         <v>0</v>
       </c>
       <c r="G20" s="10">
-        <v>42503</v>
-      </c>
-      <c r="H20" s="10"/>
+        <v>42551</v>
+      </c>
+      <c r="H20" s="10">
+        <v>42551</v>
+      </c>
       <c r="I20" s="27">
         <f t="shared" si="144"/>
-        <v>42504</v>
+        <v>42552</v>
       </c>
       <c r="J20" s="27">
         <f t="shared" si="145"/>
-        <v>-1</v>
-      </c>
-      <c r="K20" s="27" t="str">
-        <f t="shared" ca="1" si="146"/>
-        <v>Em atraso</v>
+        <v>42552</v>
+      </c>
+      <c r="K20" s="27" t="s">
+        <v>97</v>
       </c>
       <c r="L20" s="41" t="s">
         <v>34</v>
@@ -6226,7 +6479,7 @@
         <v>-1</v>
       </c>
       <c r="K21" s="27" t="str">
-        <f t="shared" ca="1" si="146"/>
+        <f t="shared" ref="K18:K46" ca="1" si="146">IF(F21=1,"Concluído",IF(AND(J21&lt;TODAY(),F21&lt;1),"Em atraso","Em andamento"))</f>
         <v>Em atraso</v>
       </c>
       <c r="L21" s="41" t="s">
@@ -6435,32 +6688,37 @@
       <c r="HE21" s="17"/>
     </row>
     <row r="22" spans="2:213" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="34"/>
+      <c r="B22" s="34">
+        <v>2</v>
+      </c>
       <c r="C22" s="39" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="34">
         <v>2</v>
       </c>
-      <c r="E22" s="34"/>
+      <c r="E22" s="34">
+        <v>2</v>
+      </c>
       <c r="F22" s="40">
         <v>0</v>
       </c>
       <c r="G22" s="10">
-        <v>42503</v>
-      </c>
-      <c r="H22" s="10"/>
+        <v>42551</v>
+      </c>
+      <c r="H22" s="10">
+        <v>42551</v>
+      </c>
       <c r="I22" s="27">
         <f t="shared" si="144"/>
-        <v>42504</v>
+        <v>42552</v>
       </c>
       <c r="J22" s="27">
         <f t="shared" si="145"/>
-        <v>-1</v>
-      </c>
-      <c r="K22" s="27" t="str">
-        <f t="shared" ca="1" si="146"/>
-        <v>Em atraso</v>
+        <v>42552</v>
+      </c>
+      <c r="K22" s="27" t="s">
+        <v>97</v>
       </c>
       <c r="L22" s="41" t="s">
         <v>34</v>
@@ -6668,32 +6926,37 @@
       <c r="HE22" s="17"/>
     </row>
     <row r="23" spans="2:213" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="34"/>
+      <c r="B23" s="34">
+        <v>2</v>
+      </c>
       <c r="C23" s="39" t="s">
         <v>43</v>
       </c>
       <c r="D23" s="34">
         <v>2</v>
       </c>
-      <c r="E23" s="34"/>
+      <c r="E23" s="34">
+        <v>2</v>
+      </c>
       <c r="F23" s="40">
         <v>0</v>
       </c>
       <c r="G23" s="10">
-        <v>42503</v>
-      </c>
-      <c r="H23" s="10"/>
+        <v>42551</v>
+      </c>
+      <c r="H23" s="10">
+        <v>42551</v>
+      </c>
       <c r="I23" s="27">
         <f t="shared" si="144"/>
-        <v>42504</v>
+        <v>42552</v>
       </c>
       <c r="J23" s="27">
         <f t="shared" si="145"/>
-        <v>-1</v>
-      </c>
-      <c r="K23" s="27" t="str">
-        <f t="shared" ca="1" si="146"/>
-        <v>Em atraso</v>
+        <v>42552</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>97</v>
       </c>
       <c r="L23" s="41" t="s">
         <v>34</v>
@@ -6901,32 +7164,37 @@
       <c r="HE23" s="17"/>
     </row>
     <row r="24" spans="2:213" ht="18.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="34"/>
+      <c r="B24" s="34">
+        <v>2</v>
+      </c>
       <c r="C24" s="39" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="34">
         <v>2</v>
       </c>
-      <c r="E24" s="34"/>
+      <c r="E24" s="34">
+        <v>2</v>
+      </c>
       <c r="F24" s="40">
         <v>0</v>
       </c>
       <c r="G24" s="10">
-        <v>42503</v>
-      </c>
-      <c r="H24" s="10"/>
+        <v>42551</v>
+      </c>
+      <c r="H24" s="10">
+        <v>42551</v>
+      </c>
       <c r="I24" s="27">
         <f t="shared" si="144"/>
-        <v>42504</v>
+        <v>42552</v>
       </c>
       <c r="J24" s="27">
         <f t="shared" si="145"/>
-        <v>-1</v>
-      </c>
-      <c r="K24" s="27" t="str">
-        <f t="shared" ca="1" si="146"/>
-        <v>Em atraso</v>
+        <v>42552</v>
+      </c>
+      <c r="K24" s="27" t="s">
+        <v>97</v>
       </c>
       <c r="L24" s="41" t="s">
         <v>34</v>
@@ -12772,11 +13040,11 @@
       <c r="AG55" s="13"/>
     </row>
     <row r="56" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="72" t="s">
+      <c r="B56" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="C56" s="72"/>
-      <c r="D56" s="72"/>
+      <c r="C56" s="73"/>
+      <c r="D56" s="73"/>
       <c r="E56" s="13"/>
       <c r="F56" s="29"/>
       <c r="G56" s="13"/>
@@ -12808,12 +13076,12 @@
       <c r="AG56" s="13"/>
     </row>
     <row r="57" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="73">
+      <c r="B57" s="74">
         <f>'Cronograma + Diagrama de Gantt'!$F$7</f>
         <v>5.128205128205128E-2</v>
       </c>
-      <c r="C57" s="73"/>
-      <c r="D57" s="73"/>
+      <c r="C57" s="74"/>
+      <c r="D57" s="74"/>
       <c r="E57" s="13"/>
       <c r="F57" s="29"/>
       <c r="G57" s="13"/>
@@ -12845,9 +13113,9 @@
       <c r="AG57" s="13"/>
     </row>
     <row r="58" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="73"/>
-      <c r="C58" s="73"/>
-      <c r="D58" s="73"/>
+      <c r="B58" s="74"/>
+      <c r="C58" s="74"/>
+      <c r="D58" s="74"/>
       <c r="E58" s="13"/>
       <c r="F58" s="29"/>
       <c r="G58" s="13"/>
@@ -12879,9 +13147,9 @@
       <c r="AG58" s="13"/>
     </row>
     <row r="59" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="73"/>
-      <c r="C59" s="73"/>
-      <c r="D59" s="73"/>
+      <c r="B59" s="74"/>
+      <c r="C59" s="74"/>
+      <c r="D59" s="74"/>
       <c r="E59" s="13"/>
       <c r="F59" s="29"/>
       <c r="G59" s="13"/>
@@ -12913,9 +13181,9 @@
       <c r="AG59" s="13"/>
     </row>
     <row r="60" spans="2:33" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="73"/>
-      <c r="C60" s="73"/>
-      <c r="D60" s="73"/>
+      <c r="B60" s="74"/>
+      <c r="C60" s="74"/>
+      <c r="D60" s="74"/>
       <c r="E60" s="13"/>
       <c r="F60" s="29"/>
       <c r="G60" s="13"/>
@@ -34108,104 +34376,181 @@
     <mergeCell ref="B57:D60"/>
   </mergeCells>
   <conditionalFormatting sqref="C48:BU48">
-    <cfRule type="expression" dxfId="26" priority="388">
+    <cfRule type="expression" dxfId="47" priority="409">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N7:HE47">
-    <cfRule type="expression" dxfId="25" priority="471">
+    <cfRule type="expression" dxfId="46" priority="492">
       <formula>PorcentagemConcluída</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="472">
+    <cfRule type="expression" dxfId="45" priority="493">
       <formula>PorcentagemConcluídaPosterior</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="473">
+    <cfRule type="expression" dxfId="44" priority="494">
       <formula>Real</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="474">
+    <cfRule type="expression" dxfId="43" priority="495">
       <formula>RealPosterior</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="475">
+    <cfRule type="expression" dxfId="42" priority="496">
       <formula>Plano</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="476">
+    <cfRule type="expression" dxfId="41" priority="497">
       <formula>N$6=$J$4+periodo_selecionado-1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="477">
+    <cfRule type="expression" dxfId="40" priority="498">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="478">
+    <cfRule type="expression" dxfId="39" priority="499">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N6:HE6">
-    <cfRule type="expression" dxfId="17" priority="479">
+    <cfRule type="expression" dxfId="38" priority="500">
       <formula>N$6=$J$4+periodo_selecionado-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV48:HE48">
-    <cfRule type="expression" dxfId="16" priority="386">
+    <cfRule type="expression" dxfId="37" priority="407">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:K10 K14 K18 K22 K26 K30 K34 K38 K42 K46:K47">
-    <cfRule type="containsText" dxfId="15" priority="379" operator="containsText" text="Em andamento">
+  <conditionalFormatting sqref="K8:K10 K14 K26 K30 K34 K38 K42 K46:K47 K18 K22">
+    <cfRule type="containsText" dxfId="36" priority="400" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",K8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="380" operator="containsText" text="Em atraso">
+    <cfRule type="containsText" dxfId="35" priority="401" operator="containsText" text="Em atraso">
       <formula>NOT(ISERROR(SEARCH("Em atraso",K8)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="381" operator="containsText" text="Concluído">
+    <cfRule type="containsText" dxfId="34" priority="402" operator="containsText" text="Concluído">
       <formula>NOT(ISERROR(SEARCH("Concluído",K8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="expression" dxfId="12" priority="378">
+    <cfRule type="expression" dxfId="33" priority="399">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K15 K19 K23 K27 K31 K35 K39 K43">
-    <cfRule type="containsText" dxfId="11" priority="367" operator="containsText" text="Em andamento">
-      <formula>NOT(ISERROR(SEARCH("Em andamento",K15)))</formula>
+  <conditionalFormatting sqref="K27 K31 K35 K39 K43">
+    <cfRule type="containsText" dxfId="32" priority="388" operator="containsText" text="Em andamento">
+      <formula>NOT(ISERROR(SEARCH("Em andamento",K27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="368" operator="containsText" text="Em atraso">
-      <formula>NOT(ISERROR(SEARCH("Em atraso",K15)))</formula>
+    <cfRule type="containsText" dxfId="31" priority="389" operator="containsText" text="Em atraso">
+      <formula>NOT(ISERROR(SEARCH("Em atraso",K27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="369" operator="containsText" text="Concluído">
-      <formula>NOT(ISERROR(SEARCH("Concluído",K15)))</formula>
+    <cfRule type="containsText" dxfId="30" priority="390" operator="containsText" text="Concluído">
+      <formula>NOT(ISERROR(SEARCH("Concluído",K27)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K12 K16 K20 K24 K28 K32 K36 K40 K44">
-    <cfRule type="containsText" dxfId="8" priority="356" operator="containsText" text="Em andamento">
+  <conditionalFormatting sqref="K12 K28 K32 K36 K40 K44">
+    <cfRule type="containsText" dxfId="29" priority="377" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="357" operator="containsText" text="Em atraso">
+    <cfRule type="containsText" dxfId="28" priority="378" operator="containsText" text="Em atraso">
       <formula>NOT(ISERROR(SEARCH("Em atraso",K12)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="358" operator="containsText" text="Concluído">
+    <cfRule type="containsText" dxfId="27" priority="379" operator="containsText" text="Concluído">
       <formula>NOT(ISERROR(SEARCH("Concluído",K12)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K13 K17 K21 K25 K29 K33 K37 K41 K45">
-    <cfRule type="containsText" dxfId="5" priority="345" operator="containsText" text="Em andamento">
+  <conditionalFormatting sqref="K13 K21 K25 K29 K33 K37 K41 K45">
+    <cfRule type="containsText" dxfId="26" priority="366" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="346" operator="containsText" text="Em atraso">
+    <cfRule type="containsText" dxfId="25" priority="367" operator="containsText" text="Em atraso">
       <formula>NOT(ISERROR(SEARCH("Em atraso",K13)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="347" operator="containsText" text="Concluído">
+    <cfRule type="containsText" dxfId="24" priority="368" operator="containsText" text="Concluído">
       <formula>NOT(ISERROR(SEARCH("Concluído",K13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Em andamento">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Em andamento">
       <formula>NOT(ISERROR(SEARCH("Em andamento",K11)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Em atraso">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="Em atraso">
       <formula>NOT(ISERROR(SEARCH("Em atraso",K11)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Concluído">
+      <formula>NOT(ISERROR(SEARCH("Concluído",K11)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Em andamento">
+      <formula>NOT(ISERROR(SEARCH("Em andamento",K15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Em atraso">
+      <formula>NOT(ISERROR(SEARCH("Em atraso",K15)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Concluído">
+      <formula>NOT(ISERROR(SEARCH("Concluído",K15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Em andamento">
+      <formula>NOT(ISERROR(SEARCH("Em andamento",K16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Em atraso">
+      <formula>NOT(ISERROR(SEARCH("Em atraso",K16)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Concluído">
+      <formula>NOT(ISERROR(SEARCH("Concluído",K16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="Em andamento">
+      <formula>NOT(ISERROR(SEARCH("Em andamento",K17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Em atraso">
+      <formula>NOT(ISERROR(SEARCH("Em atraso",K17)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Concluído">
+      <formula>NOT(ISERROR(SEARCH("Concluído",K17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Em andamento">
+      <formula>NOT(ISERROR(SEARCH("Em andamento",K19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Em atraso">
+      <formula>NOT(ISERROR(SEARCH("Em atraso",K19)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Concluído">
+      <formula>NOT(ISERROR(SEARCH("Concluído",K19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K20">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Em andamento">
+      <formula>NOT(ISERROR(SEARCH("Em andamento",K20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Em atraso">
+      <formula>NOT(ISERROR(SEARCH("Em atraso",K20)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Concluído">
+      <formula>NOT(ISERROR(SEARCH("Concluído",K20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Em andamento">
+      <formula>NOT(ISERROR(SEARCH("Em andamento",K23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Em atraso">
+      <formula>NOT(ISERROR(SEARCH("Em atraso",K23)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Concluído">
+      <formula>NOT(ISERROR(SEARCH("Concluído",K23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K24">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Em andamento">
+      <formula>NOT(ISERROR(SEARCH("Em andamento",K24)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Em atraso">
+      <formula>NOT(ISERROR(SEARCH("Em atraso",K24)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Concluído">
-      <formula>NOT(ISERROR(SEARCH("Concluído",K11)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Concluído",K24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -34252,8 +34597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34278,55 +34623,55 @@
         <v>29</v>
       </c>
       <c r="D1" s="57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E1" s="57"/>
       <c r="F1" s="57"/>
       <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
+      <c r="A3" s="76"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
     </row>
     <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
+      <c r="A4" s="76"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="75"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="63" t="s">
@@ -34345,7 +34690,7 @@
         <v>72</v>
       </c>
       <c r="F6" s="64" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G6" s="64" t="s">
         <v>73</v>
@@ -34356,10 +34701,10 @@
         <v>75</v>
       </c>
       <c r="B7" s="67" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="69">
         <v>42503</v>
@@ -34371,7 +34716,7 @@
         <v>42506</v>
       </c>
       <c r="G7" s="68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -34379,10 +34724,10 @@
         <v>76</v>
       </c>
       <c r="B8" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="68" t="s">
         <v>84</v>
-      </c>
-      <c r="C8" s="68" t="s">
-        <v>85</v>
       </c>
       <c r="D8" s="69">
         <v>42503</v>
@@ -34394,7 +34739,7 @@
         <v>42505</v>
       </c>
       <c r="G8" s="68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -34402,10 +34747,10 @@
         <v>77</v>
       </c>
       <c r="B9" s="67" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="69">
         <v>42505</v>
@@ -34417,7 +34762,7 @@
         <v>42510</v>
       </c>
       <c r="G9" s="68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -34425,10 +34770,10 @@
         <v>78</v>
       </c>
       <c r="B10" s="67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="68" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="69">
         <v>42505</v>
@@ -34440,7 +34785,7 @@
         <v>42510</v>
       </c>
       <c r="G10" s="68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -34448,10 +34793,10 @@
         <v>79</v>
       </c>
       <c r="B11" s="67" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="68" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11" s="69">
         <v>42507</v>
@@ -34463,7 +34808,7 @@
         <v>42510</v>
       </c>
       <c r="G11" s="68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -34471,7 +34816,7 @@
         <v>80</v>
       </c>
       <c r="B12" s="67" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" s="68" t="s">
         <v>26</v>
@@ -34486,7 +34831,7 @@
         <v>42510</v>
       </c>
       <c r="G12" s="68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -34494,7 +34839,7 @@
         <v>80</v>
       </c>
       <c r="B13" s="67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C13" s="68" t="s">
         <v>25</v>
@@ -34509,7 +34854,7 @@
         <v>42510</v>
       </c>
       <c r="G13" s="68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -34517,7 +34862,7 @@
         <v>81</v>
       </c>
       <c r="B14" s="67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C14" s="68" t="s">
         <v>25</v>
@@ -34532,7 +34877,7 @@
         <v>42510</v>
       </c>
       <c r="G14" s="68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -34563,8 +34908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34583,61 +34928,61 @@
         <v>28</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" s="56" t="s">
         <v>29</v>
       </c>
       <c r="D1" s="57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E1" s="57"/>
       <c r="F1" s="57"/>
       <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="74" t="s">
-        <v>100</v>
-      </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
+      <c r="A2" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="75"/>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
+      <c r="A3" s="76"/>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
     </row>
     <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="75"/>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
+      <c r="A4" s="76"/>
+      <c r="B4" s="76"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="75"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="76"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="63"/>
@@ -34653,10 +34998,10 @@
         <v>75</v>
       </c>
       <c r="B7" s="60" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C7" s="62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" s="61">
         <v>42513</v>
@@ -34664,11 +35009,11 @@
       <c r="E7" s="61">
         <v>42518</v>
       </c>
-      <c r="F7" s="61">
+      <c r="F7" s="77">
         <v>42518</v>
       </c>
       <c r="G7" s="62" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -34676,10 +35021,10 @@
         <v>76</v>
       </c>
       <c r="B8" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="C8" s="76" t="s">
-        <v>111</v>
+        <v>115</v>
+      </c>
+      <c r="C8" s="71" t="s">
+        <v>109</v>
       </c>
       <c r="D8" s="61">
         <v>42517</v>
@@ -34687,11 +35032,11 @@
       <c r="E8" s="61">
         <v>42517</v>
       </c>
-      <c r="F8" s="61">
+      <c r="F8" s="77">
         <v>42517</v>
       </c>
       <c r="G8" s="62" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="75" x14ac:dyDescent="0.25">
@@ -34699,10 +35044,10 @@
         <v>77</v>
       </c>
       <c r="B9" s="60" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C9" s="62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="61">
         <v>42519</v>
@@ -34710,9 +35055,11 @@
       <c r="E9" s="61">
         <v>42519</v>
       </c>
-      <c r="F9" s="61"/>
+      <c r="F9" s="77">
+        <v>42519</v>
+      </c>
       <c r="G9" s="62" t="s">
-        <v>82</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -34720,10 +35067,10 @@
         <v>78</v>
       </c>
       <c r="B10" s="60" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C10" s="62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="61">
         <v>42520</v>
@@ -34731,9 +35078,11 @@
       <c r="E10" s="61">
         <v>42522</v>
       </c>
-      <c r="F10" s="61"/>
+      <c r="F10" s="77">
+        <v>42522</v>
+      </c>
       <c r="G10" s="62" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -34741,10 +35090,10 @@
         <v>79</v>
       </c>
       <c r="B11" s="60" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C11" s="62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="61">
         <v>42520</v>
@@ -34752,9 +35101,11 @@
       <c r="E11" s="61">
         <v>42523</v>
       </c>
-      <c r="F11" s="61"/>
+      <c r="F11" s="77">
+        <v>42523</v>
+      </c>
       <c r="G11" s="62" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -34762,10 +35113,10 @@
         <v>80</v>
       </c>
       <c r="B12" s="60" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C12" s="62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="61">
         <v>42520</v>
@@ -34773,9 +35124,11 @@
       <c r="E12" s="61">
         <v>42521</v>
       </c>
-      <c r="F12" s="61"/>
+      <c r="F12" s="77">
+        <v>42521</v>
+      </c>
       <c r="G12" s="62" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -34783,10 +35136,10 @@
         <v>81</v>
       </c>
       <c r="B13" s="60" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13" s="62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="61">
         <v>42522</v>
@@ -34794,20 +35147,22 @@
       <c r="E13" s="61">
         <v>42523</v>
       </c>
-      <c r="F13" s="61"/>
+      <c r="F13" s="77">
+        <v>42523</v>
+      </c>
       <c r="G13" s="62" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="65" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B14" s="60" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C14" s="62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D14" s="61">
         <v>42523</v>
@@ -34815,17 +35170,19 @@
       <c r="E14" s="61">
         <v>42524</v>
       </c>
-      <c r="F14" s="61"/>
+      <c r="F14" s="77">
+        <v>42524</v>
+      </c>
       <c r="G14" s="62" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A15" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B15" s="60" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C15" s="62" t="s">
         <v>26</v>
@@ -34836,20 +35193,22 @@
       <c r="E15" s="61">
         <v>42524</v>
       </c>
-      <c r="F15" s="61"/>
+      <c r="F15" s="77">
+        <v>42524</v>
+      </c>
       <c r="G15" s="62" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="65" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B16" s="60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" s="62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" s="61">
         <v>42524</v>
@@ -34857,20 +35216,22 @@
       <c r="E16" s="61">
         <v>42524</v>
       </c>
-      <c r="F16" s="61"/>
+      <c r="F16" s="78">
+        <v>42525</v>
+      </c>
       <c r="G16" s="62" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="65" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B17" s="60" t="s">
-        <v>112</v>
-      </c>
-      <c r="C17" s="76" t="s">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="C17" s="71" t="s">
+        <v>109</v>
       </c>
       <c r="D17" s="61">
         <v>42524</v>
@@ -34878,20 +35239,22 @@
       <c r="E17" s="61">
         <v>42524</v>
       </c>
-      <c r="F17" s="61"/>
+      <c r="F17" s="78">
+        <v>42526</v>
+      </c>
       <c r="G17" s="62" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="65" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B18" s="60" t="s">
-        <v>114</v>
-      </c>
-      <c r="C18" s="76" t="s">
-        <v>120</v>
+        <v>112</v>
+      </c>
+      <c r="C18" s="71" t="s">
+        <v>118</v>
       </c>
       <c r="D18" s="61">
         <v>42524</v>
@@ -34899,9 +35262,11 @@
       <c r="E18" s="61">
         <v>42524</v>
       </c>
-      <c r="F18" s="61"/>
+      <c r="F18" s="78">
+        <v>42527</v>
+      </c>
       <c r="G18" s="62" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>